<commit_message>
Styling and fixing explore page
</commit_message>
<xml_diff>
--- a/public/upload/categories.xlsx
+++ b/public/upload/categories.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="569">
   <si>
     <t>Category</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Alias</t>
+  </si>
+  <si>
+    <t>ka</t>
+  </si>
+  <si>
+    <t>ru</t>
   </si>
   <si>
     <t>Income</t>
@@ -1820,10 +1826,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J263"/>
+  <dimension ref="A1:L263"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A208" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J241" activeCellId="0" sqref="J241"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.95"/>
@@ -1864,42 +1870,48 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -1909,18 +1921,18 @@
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>2</v>
@@ -1931,18 +1943,18 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>3</v>
@@ -1954,17 +1966,17 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="1"/>
@@ -1974,14 +1986,14 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1991,15 +2003,15 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="1" t="n">
@@ -2012,14 +2024,14 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -2030,14 +2042,14 @@
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -2047,15 +2059,15 @@
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1" t="n">
@@ -2068,14 +2080,14 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2086,14 +2098,14 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -2104,14 +2116,14 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -2122,14 +2134,14 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -2139,15 +2151,15 @@
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="1" t="n">
@@ -2159,15 +2171,15 @@
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="1" t="n">
@@ -2178,16 +2190,16 @@
     <row r="18" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -2197,18 +2209,18 @@
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I19" s="1" t="n">
         <v>5</v>
@@ -2220,17 +2232,17 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="1"/>
@@ -2240,17 +2252,17 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="1"/>
@@ -2260,14 +2272,14 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -2277,15 +2289,15 @@
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="1" t="n">
@@ -2295,14 +2307,14 @@
     </row>
     <row r="24" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G24" s="1" t="n">
         <v>1</v>
@@ -2312,19 +2324,19 @@
         <v>6</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G25" s="1" t="n">
         <v>1.1</v>
@@ -2337,18 +2349,18 @@
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I26" s="1" t="n">
         <v>7</v>
@@ -2359,18 +2371,18 @@
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I27" s="1" t="n">
         <v>8</v>
@@ -2382,17 +2394,17 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="1"/>
@@ -2402,14 +2414,14 @@
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -2419,15 +2431,15 @@
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="1" t="n">
@@ -2440,14 +2452,14 @@
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -2458,14 +2470,14 @@
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -2475,15 +2487,15 @@
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="1" t="n">
@@ -2496,14 +2508,14 @@
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -2514,14 +2526,14 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -2532,14 +2544,14 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -2550,14 +2562,14 @@
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -2567,15 +2579,15 @@
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="1" t="n">
@@ -2587,15 +2599,15 @@
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="1" t="n">
@@ -2606,13 +2618,13 @@
     <row r="40" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2"/>
       <c r="B40" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G40" s="1" t="n">
         <v>1.2</v>
@@ -2625,18 +2637,18 @@
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I41" s="1" t="n">
         <v>10</v>
@@ -2648,17 +2660,17 @@
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="1"/>
@@ -2668,17 +2680,17 @@
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="1"/>
@@ -2688,14 +2700,14 @@
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -2705,15 +2717,15 @@
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="1" t="n">
@@ -2746,42 +2758,42 @@
     </row>
     <row r="48" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="1" t="n">
         <v>11</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="2"/>
       <c r="B49" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I49" s="1" t="n">
         <v>12</v>
@@ -2791,18 +2803,18 @@
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="I50" s="2"/>
     </row>
@@ -2810,15 +2822,15 @@
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
@@ -2826,16 +2838,16 @@
     <row r="52" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="2"/>
       <c r="B52" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
@@ -2844,15 +2856,15 @@
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="1" t="n">
@@ -2864,17 +2876,17 @@
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I54" s="2"/>
     </row>
@@ -2883,17 +2895,17 @@
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I55" s="2"/>
     </row>
@@ -2901,15 +2913,15 @@
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="1" t="n">
@@ -2921,14 +2933,14 @@
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
@@ -2938,14 +2950,14 @@
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
@@ -2955,14 +2967,14 @@
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
@@ -2972,14 +2984,14 @@
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
@@ -2989,14 +3001,14 @@
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
@@ -3006,14 +3018,14 @@
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
@@ -3024,13 +3036,13 @@
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
@@ -3041,13 +3053,13 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
@@ -3058,13 +3070,13 @@
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -3075,13 +3087,13 @@
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -3091,14 +3103,14 @@
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
@@ -3107,15 +3119,15 @@
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="1" t="n">
@@ -3126,15 +3138,15 @@
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="1" t="n">
@@ -3145,15 +3157,15 @@
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="1" t="n">
@@ -3164,15 +3176,15 @@
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="1" t="n">
@@ -3184,14 +3196,14 @@
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -3201,14 +3213,14 @@
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
@@ -3217,15 +3229,15 @@
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="1" t="n">
@@ -3236,15 +3248,15 @@
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="1" t="n">
@@ -3256,14 +3268,14 @@
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -3273,14 +3285,14 @@
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -3290,14 +3302,14 @@
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -3307,14 +3319,14 @@
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
@@ -3324,14 +3336,14 @@
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
@@ -3340,15 +3352,15 @@
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H81" s="2"/>
       <c r="I81" s="1" t="n">
@@ -3359,15 +3371,15 @@
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H82" s="2"/>
       <c r="I82" s="1" t="n">
@@ -3378,15 +3390,15 @@
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="H83" s="2"/>
       <c r="I83" s="1" t="n">
@@ -3397,15 +3409,15 @@
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="H84" s="2"/>
       <c r="I84" s="1" t="n">
@@ -3416,15 +3428,15 @@
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="1" t="n">
@@ -3436,17 +3448,17 @@
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="I86" s="2"/>
     </row>
@@ -3455,17 +3467,17 @@
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="I87" s="2"/>
     </row>
@@ -3474,17 +3486,17 @@
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="I88" s="2"/>
     </row>
@@ -3492,15 +3504,15 @@
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
       <c r="F89" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="H89" s="2"/>
       <c r="I89" s="1" t="n">
@@ -3511,15 +3523,15 @@
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
       <c r="F90" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H90" s="2"/>
       <c r="I90" s="1" t="n">
@@ -3529,19 +3541,19 @@
     <row r="91" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="2"/>
       <c r="B91" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="I91" s="1" t="n">
         <v>99</v>
@@ -3551,15 +3563,15 @@
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
@@ -3568,15 +3580,15 @@
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
@@ -3584,16 +3596,16 @@
     <row r="94" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="2"/>
       <c r="B94" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="H94" s="2"/>
       <c r="I94" s="1" t="n">
@@ -3603,16 +3615,16 @@
     <row r="95" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="2"/>
       <c r="B95" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="1" t="n">
@@ -3622,16 +3634,16 @@
     <row r="96" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="2"/>
       <c r="B96" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="H96" s="2"/>
       <c r="I96" s="1" t="n">
@@ -3642,15 +3654,15 @@
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
       <c r="F97" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
@@ -3659,15 +3671,15 @@
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
       <c r="F98" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
@@ -3676,15 +3688,15 @@
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
       <c r="F99" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
@@ -3693,15 +3705,15 @@
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
@@ -3710,15 +3722,15 @@
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
@@ -3726,16 +3738,16 @@
     <row r="102" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="2"/>
       <c r="B102" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="H102" s="2"/>
       <c r="I102" s="1" t="n">
@@ -3746,15 +3758,15 @@
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
@@ -3763,12 +3775,12 @@
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="G104" s="1" t="n">
         <v>2.2</v>
@@ -3780,15 +3792,15 @@
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
@@ -3797,15 +3809,15 @@
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
@@ -3814,15 +3826,15 @@
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
@@ -3831,15 +3843,15 @@
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
@@ -3848,15 +3860,15 @@
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
@@ -3864,16 +3876,16 @@
     <row r="110" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="2"/>
       <c r="B110" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="H110" s="2"/>
       <c r="I110" s="1" t="n">
@@ -3883,16 +3895,16 @@
     <row r="111" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="2"/>
       <c r="B111" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="H111" s="2"/>
       <c r="I111" s="1" t="n">
@@ -3903,15 +3915,15 @@
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
@@ -3920,15 +3932,15 @@
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
@@ -3936,16 +3948,16 @@
     <row r="114" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="2"/>
       <c r="B114" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="H114" s="2"/>
       <c r="I114" s="1" t="n">
@@ -3976,14 +3988,14 @@
     </row>
     <row r="117" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="G117" s="1" t="n">
         <v>1</v>
@@ -3993,19 +4005,19 @@
         <v>16</v>
       </c>
       <c r="J117" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="2"/>
       <c r="B118" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="1" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="G118" s="1" t="n">
         <v>1.1</v>
@@ -4019,15 +4031,15 @@
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
@@ -4036,15 +4048,15 @@
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
@@ -4052,13 +4064,13 @@
     <row r="121" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="2"/>
       <c r="B121" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="G121" s="1" t="n">
         <v>1.2</v>
@@ -4070,15 +4082,15 @@
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="H122" s="2"/>
       <c r="I122" s="1" t="n">
@@ -4090,14 +4102,14 @@
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E123" s="2"/>
       <c r="F123" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
@@ -4107,14 +4119,14 @@
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E124" s="2"/>
       <c r="F124" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
@@ -4123,15 +4135,15 @@
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H125" s="2"/>
       <c r="I125" s="1" t="n">
@@ -4143,14 +4155,14 @@
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E126" s="2"/>
       <c r="F126" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
@@ -4160,14 +4172,14 @@
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E127" s="2"/>
       <c r="F127" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
@@ -4177,14 +4189,14 @@
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E128" s="2"/>
       <c r="F128" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
@@ -4194,14 +4206,14 @@
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E129" s="2"/>
       <c r="F129" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
@@ -4211,14 +4223,14 @@
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
@@ -4228,14 +4240,14 @@
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E131" s="2"/>
       <c r="F131" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
@@ -4246,13 +4258,13 @@
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
       <c r="E132" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
@@ -4263,13 +4275,13 @@
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
       <c r="E133" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
@@ -4280,13 +4292,13 @@
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
       <c r="E134" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="H134" s="2"/>
       <c r="I134" s="2"/>
@@ -4297,13 +4309,13 @@
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
       <c r="E135" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
@@ -4313,14 +4325,14 @@
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="H136" s="2"/>
       <c r="I136" s="2"/>
@@ -4329,15 +4341,15 @@
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D137" s="2"/>
       <c r="E137" s="2"/>
       <c r="F137" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="H137" s="2"/>
       <c r="I137" s="1" t="n">
@@ -4348,15 +4360,15 @@
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
       <c r="F138" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="H138" s="2"/>
       <c r="I138" s="1" t="n">
@@ -4367,15 +4379,15 @@
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
       <c r="F139" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="H139" s="2"/>
       <c r="I139" s="1" t="n">
@@ -4386,15 +4398,15 @@
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
       <c r="F140" s="1" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="H140" s="2"/>
       <c r="I140" s="1" t="n">
@@ -4406,14 +4418,14 @@
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E141" s="2"/>
       <c r="F141" s="1" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="H141" s="2"/>
       <c r="I141" s="2"/>
@@ -4423,14 +4435,14 @@
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E142" s="2"/>
       <c r="F142" s="1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="H142" s="2"/>
       <c r="I142" s="2"/>
@@ -4439,15 +4451,15 @@
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D143" s="2"/>
       <c r="E143" s="2"/>
       <c r="F143" s="1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="H143" s="2"/>
       <c r="I143" s="1" t="n">
@@ -4458,15 +4470,15 @@
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
       <c r="F144" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="H144" s="2"/>
       <c r="I144" s="1" t="n">
@@ -4478,14 +4490,14 @@
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E145" s="2"/>
       <c r="F145" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="H145" s="2"/>
       <c r="I145" s="2"/>
@@ -4495,14 +4507,14 @@
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E146" s="2"/>
       <c r="F146" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="H146" s="2"/>
       <c r="I146" s="2"/>
@@ -4512,14 +4524,14 @@
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E147" s="2"/>
       <c r="F147" s="1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="H147" s="2"/>
       <c r="I147" s="2"/>
@@ -4529,14 +4541,14 @@
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E148" s="2"/>
       <c r="F148" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="H148" s="2"/>
       <c r="I148" s="2"/>
@@ -4546,14 +4558,14 @@
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E149" s="2"/>
       <c r="F149" s="1" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="H149" s="2"/>
       <c r="I149" s="2"/>
@@ -4562,15 +4574,15 @@
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
       <c r="F150" s="1" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="H150" s="2"/>
       <c r="I150" s="1" t="n">
@@ -4581,15 +4593,15 @@
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
       <c r="F151" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="H151" s="2"/>
       <c r="I151" s="1" t="n">
@@ -4600,15 +4612,15 @@
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
       <c r="F152" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="H152" s="2"/>
       <c r="I152" s="1" t="n">
@@ -4619,15 +4631,15 @@
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
       <c r="F153" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="H153" s="2"/>
       <c r="I153" s="1" t="n">
@@ -4638,15 +4650,15 @@
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
       <c r="F154" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="H154" s="2"/>
       <c r="I154" s="1" t="n">
@@ -4658,14 +4670,14 @@
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
       <c r="D155" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E155" s="2"/>
       <c r="F155" s="1" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="H155" s="2"/>
       <c r="I155" s="2"/>
@@ -4675,14 +4687,14 @@
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
       <c r="D156" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E156" s="2"/>
       <c r="F156" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H156" s="2"/>
       <c r="I156" s="2"/>
@@ -4692,14 +4704,14 @@
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
       <c r="D157" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E157" s="2"/>
       <c r="F157" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="H157" s="2"/>
       <c r="I157" s="2"/>
@@ -4708,15 +4720,15 @@
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
       <c r="F158" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="H158" s="2"/>
       <c r="I158" s="1" t="n">
@@ -4727,15 +4739,15 @@
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D159" s="2"/>
       <c r="E159" s="2"/>
       <c r="F159" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="H159" s="2"/>
       <c r="I159" s="1" t="n">
@@ -4745,13 +4757,13 @@
     <row r="160" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="2"/>
       <c r="B160" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C160" s="2"/>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
       <c r="F160" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="G160" s="1" t="n">
         <v>1.3</v>
@@ -4765,15 +4777,15 @@
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
       <c r="C161" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
       <c r="F161" s="1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="H161" s="2"/>
       <c r="I161" s="2"/>
@@ -4782,15 +4794,15 @@
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
       <c r="F162" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="H162" s="2"/>
       <c r="I162" s="2"/>
@@ -4798,13 +4810,13 @@
     <row r="163" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="2"/>
       <c r="B163" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
       <c r="F163" s="1" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="G163" s="1" t="n">
         <v>1.4</v>
@@ -4817,13 +4829,13 @@
     <row r="164" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="2"/>
       <c r="B164" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
       <c r="F164" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="G164" s="1" t="n">
         <v>1.5</v>
@@ -4836,13 +4848,13 @@
     <row r="165" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="2"/>
       <c r="B165" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C165" s="2"/>
       <c r="D165" s="2"/>
       <c r="E165" s="2"/>
       <c r="F165" s="1" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="G165" s="1" t="n">
         <v>1.6</v>
@@ -4856,15 +4868,15 @@
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D166" s="2"/>
       <c r="E166" s="2"/>
       <c r="F166" s="1" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="H166" s="2"/>
       <c r="I166" s="2"/>
@@ -4873,15 +4885,15 @@
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
       <c r="C167" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
       <c r="F167" s="1" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="H167" s="2"/>
       <c r="I167" s="2"/>
@@ -4890,15 +4902,15 @@
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
       <c r="C168" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
       <c r="F168" s="1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="H168" s="2"/>
       <c r="I168" s="2"/>
@@ -4907,15 +4919,15 @@
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
       <c r="C169" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
       <c r="F169" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="H169" s="2"/>
       <c r="I169" s="2"/>
@@ -4924,15 +4936,15 @@
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
       <c r="C170" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
       <c r="F170" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="H170" s="2"/>
       <c r="I170" s="2"/>
@@ -4940,13 +4952,13 @@
     <row r="171" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="2"/>
       <c r="B171" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
       <c r="F171" s="1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="G171" s="1" t="n">
         <v>2</v>
@@ -4960,12 +4972,12 @@
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
       <c r="F172" s="1" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="G172" s="1" t="n">
         <v>2.1</v>
@@ -4977,12 +4989,12 @@
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D173" s="2"/>
       <c r="E173" s="2"/>
       <c r="F173" s="1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="G173" s="1" t="n">
         <v>2.2</v>
@@ -4994,12 +5006,12 @@
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
       <c r="F174" s="1" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="G174" s="1" t="n">
         <v>2.3</v>
@@ -5011,12 +5023,12 @@
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
       <c r="F175" s="1" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="G175" s="1" t="n">
         <v>2.4</v>
@@ -5028,12 +5040,12 @@
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
       <c r="F176" s="1" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="G176" s="1" t="n">
         <v>2.5</v>
@@ -5045,12 +5057,12 @@
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
       <c r="F177" s="1" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G177" s="1" t="n">
         <v>2.6</v>
@@ -5061,13 +5073,13 @@
     <row r="178" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="2"/>
       <c r="B178" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C178" s="2"/>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
       <c r="F178" s="1" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="G178" s="1" t="n">
         <v>3</v>
@@ -5080,13 +5092,13 @@
     <row r="179" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="2"/>
       <c r="B179" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
       <c r="F179" s="1" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="G179" s="1" t="n">
         <v>4</v>
@@ -5100,12 +5112,12 @@
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
       <c r="F180" s="1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="G180" s="1" t="n">
         <v>4.1</v>
@@ -5117,12 +5129,12 @@
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
       <c r="F181" s="1" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="G181" s="1" t="n">
         <v>4.2</v>
@@ -5133,13 +5145,13 @@
     <row r="182" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="2"/>
       <c r="B182" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
       <c r="F182" s="1" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="G182" s="1" t="n">
         <v>5</v>
@@ -5152,13 +5164,13 @@
     <row r="183" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="2"/>
       <c r="B183" s="1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
       <c r="F183" s="1" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="G183" s="1" t="n">
         <v>6</v>
@@ -5172,12 +5184,12 @@
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="1" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
       <c r="F184" s="1" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="G184" s="1" t="n">
         <v>6.1</v>
@@ -5189,12 +5201,12 @@
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
       <c r="F185" s="1" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="G185" s="1" t="n">
         <v>6.2</v>
@@ -5206,12 +5218,12 @@
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
       <c r="F186" s="1" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="G186" s="1" t="n">
         <v>6.3</v>
@@ -5223,12 +5235,12 @@
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
       <c r="F187" s="1" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="G187" s="1" t="n">
         <v>6.4</v>
@@ -5240,12 +5252,12 @@
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D188" s="2"/>
       <c r="E188" s="2"/>
       <c r="F188" s="1" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="G188" s="1" t="n">
         <v>6.5</v>
@@ -5257,12 +5269,12 @@
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
       <c r="F189" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="G189" s="1" t="n">
         <v>6.6</v>
@@ -5294,42 +5306,42 @@
     </row>
     <row r="192" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
       <c r="E192" s="2"/>
       <c r="F192" s="1" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="G192" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H192" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I192" s="2"/>
       <c r="J192" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="2"/>
       <c r="B193" s="1" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
       <c r="E193" s="2"/>
       <c r="F193" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="G193" s="1" t="n">
         <v>1.1</v>
       </c>
       <c r="H193" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I193" s="2"/>
     </row>
@@ -5337,18 +5349,18 @@
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
       <c r="C194" s="1" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
       <c r="F194" s="1" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H194" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I194" s="2"/>
     </row>
@@ -5356,37 +5368,37 @@
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
       <c r="C195" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D195" s="2"/>
       <c r="E195" s="2"/>
       <c r="F195" s="1" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="G195" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H195" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I195" s="2"/>
     </row>
     <row r="196" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="2"/>
       <c r="B196" s="1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C196" s="2"/>
       <c r="D196" s="2"/>
       <c r="E196" s="2"/>
       <c r="F196" s="1" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="G196" s="1" t="n">
         <v>1.2</v>
       </c>
       <c r="H196" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I196" s="2"/>
     </row>
@@ -5394,18 +5406,18 @@
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
       <c r="C197" s="1" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D197" s="2"/>
       <c r="E197" s="2"/>
       <c r="F197" s="1" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="G197" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H197" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I197" s="2"/>
     </row>
@@ -5413,37 +5425,37 @@
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D198" s="2"/>
       <c r="E198" s="2"/>
       <c r="F198" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="G198" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H198" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I198" s="2"/>
     </row>
     <row r="199" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="2"/>
       <c r="B199" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
       <c r="E199" s="2"/>
       <c r="F199" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="G199" s="1" t="n">
         <v>1.3</v>
       </c>
       <c r="H199" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I199" s="2"/>
     </row>
@@ -5451,18 +5463,18 @@
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
       <c r="C200" s="1" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
       <c r="F200" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="G200" s="1" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="H200" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I200" s="2"/>
     </row>
@@ -5470,75 +5482,75 @@
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
       <c r="C201" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D201" s="2"/>
       <c r="E201" s="2"/>
       <c r="F201" s="1" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="G201" s="1" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="H201" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I201" s="2"/>
     </row>
     <row r="202" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="2"/>
       <c r="B202" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C202" s="2"/>
       <c r="D202" s="2"/>
       <c r="E202" s="2"/>
       <c r="F202" s="1" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="G202" s="1" t="n">
         <v>1.4</v>
       </c>
       <c r="H202" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I202" s="2"/>
     </row>
     <row r="203" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="2"/>
       <c r="B203" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
       <c r="E203" s="2"/>
       <c r="F203" s="1" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="G203" s="1" t="n">
         <v>1.5</v>
       </c>
       <c r="H203" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I203" s="2"/>
     </row>
     <row r="204" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="2"/>
       <c r="B204" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C204" s="2"/>
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
       <c r="F204" s="1" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="G204" s="1" t="n">
         <v>1.6</v>
       </c>
       <c r="H204" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I204" s="2"/>
     </row>
@@ -5571,7 +5583,7 @@
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
       <c r="F207" s="1" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="G207" s="2"/>
       <c r="H207" s="2"/>
@@ -5579,14 +5591,14 @@
     </row>
     <row r="208" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
       <c r="F208" s="1" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="G208" s="2"/>
       <c r="H208" s="2"/>
@@ -5594,25 +5606,25 @@
         <v>21</v>
       </c>
       <c r="J208" s="0" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="2"/>
       <c r="B209" s="1" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
       <c r="E209" s="2"/>
       <c r="F209" s="1" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="G209" s="1" t="n">
         <v>1110</v>
       </c>
       <c r="H209" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="I209" s="1" t="n">
         <v>22</v>
@@ -5621,13 +5633,13 @@
     <row r="210" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="2"/>
       <c r="B210" s="1" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
       <c r="E210" s="2"/>
       <c r="F210" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="G210" s="1" t="n">
         <v>1120</v>
@@ -5640,19 +5652,19 @@
     <row r="211" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="2"/>
       <c r="B211" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
       <c r="E211" s="2"/>
       <c r="F211" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="G211" s="1" t="n">
         <v>1211</v>
       </c>
       <c r="H211" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I211" s="1" t="n">
         <v>24</v>
@@ -5661,19 +5673,19 @@
     <row r="212" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="2"/>
       <c r="B212" s="1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
       <c r="E212" s="2"/>
       <c r="F212" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="G212" s="1" t="n">
         <v>1212</v>
       </c>
       <c r="H212" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I212" s="1" t="n">
         <v>25</v>
@@ -5682,19 +5694,19 @@
     <row r="213" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="2"/>
       <c r="B213" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
       <c r="E213" s="2"/>
       <c r="F213" s="1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="G213" s="1" t="n">
         <v>1213</v>
       </c>
       <c r="H213" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I213" s="1" t="n">
         <v>26</v>
@@ -5703,19 +5715,19 @@
     <row r="214" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="2"/>
       <c r="B214" s="1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
       <c r="E214" s="2"/>
       <c r="F214" s="1" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="G214" s="1" t="n">
         <v>1214</v>
       </c>
       <c r="H214" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I214" s="1" t="n">
         <v>27</v>
@@ -5724,19 +5736,19 @@
     <row r="215" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="2"/>
       <c r="B215" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
       <c r="E215" s="2"/>
       <c r="F215" s="1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="G215" s="1" t="n">
         <v>1215</v>
       </c>
       <c r="H215" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I215" s="1" t="n">
         <v>99</v>
@@ -5745,13 +5757,13 @@
     <row r="216" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="2"/>
       <c r="B216" s="1" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
       <c r="E216" s="2"/>
       <c r="F216" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="G216" s="1" t="n">
         <v>1300</v>
@@ -5764,13 +5776,13 @@
     <row r="217" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="2"/>
       <c r="B217" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
       <c r="E217" s="2"/>
       <c r="F217" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="G217" s="1" t="n">
         <v>1410</v>
@@ -5783,13 +5795,13 @@
     <row r="218" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="2"/>
       <c r="B218" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
       <c r="E218" s="2"/>
       <c r="F218" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="G218" s="1" t="n">
         <v>1421</v>
@@ -5802,13 +5814,13 @@
     <row r="219" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="2"/>
       <c r="B219" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
       <c r="E219" s="2"/>
       <c r="F219" s="1" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="G219" s="1" t="n">
         <v>1422</v>
@@ -5821,13 +5833,13 @@
     <row r="220" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="2"/>
       <c r="B220" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
       <c r="E220" s="2"/>
       <c r="F220" s="1" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="G220" s="1" t="n">
         <v>1423</v>
@@ -5840,13 +5852,13 @@
     <row r="221" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="2"/>
       <c r="B221" s="1" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
       <c r="F221" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="G221" s="1" t="n">
         <v>1431</v>
@@ -5859,13 +5871,13 @@
     <row r="222" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="2"/>
       <c r="B222" s="1" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
       <c r="E222" s="2"/>
       <c r="F222" s="1" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="G222" s="1" t="n">
         <v>1432</v>
@@ -5878,13 +5890,13 @@
     <row r="223" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="2"/>
       <c r="B223" s="1" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C223" s="2"/>
       <c r="D223" s="2"/>
       <c r="E223" s="2"/>
       <c r="F223" s="1" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="G223" s="1" t="n">
         <v>1433</v>
@@ -5897,13 +5909,13 @@
     <row r="224" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="2"/>
       <c r="B224" s="1" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
       <c r="E224" s="2"/>
       <c r="F224" s="1" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="G224" s="1" t="n">
         <v>1441</v>
@@ -5916,13 +5928,13 @@
     <row r="225" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="2"/>
       <c r="B225" s="1" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
       <c r="E225" s="2"/>
       <c r="F225" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="G225" s="1" t="n">
         <v>1442</v>
@@ -5935,13 +5947,13 @@
     <row r="226" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="2"/>
       <c r="B226" s="1" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C226" s="2"/>
       <c r="D226" s="2"/>
       <c r="E226" s="2"/>
       <c r="F226" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="G226" s="1" t="n">
         <v>1443</v>
@@ -5954,13 +5966,13 @@
     <row r="227" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="2"/>
       <c r="B227" s="1" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C227" s="2"/>
       <c r="D227" s="2"/>
       <c r="E227" s="2"/>
       <c r="F227" s="1" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="G227" s="1" t="n">
         <v>1444</v>
@@ -5973,13 +5985,13 @@
     <row r="228" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="2"/>
       <c r="B228" s="1" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
       <c r="E228" s="2"/>
       <c r="F228" s="1" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="G228" s="1" t="n">
         <v>1445</v>
@@ -5992,13 +6004,13 @@
     <row r="229" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="2"/>
       <c r="B229" s="1" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
       <c r="E229" s="2"/>
       <c r="F229" s="1" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="G229" s="1" t="n">
         <v>1446</v>
@@ -6010,42 +6022,42 @@
     </row>
     <row r="230" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
       <c r="D230" s="2"/>
       <c r="E230" s="2"/>
       <c r="F230" s="1" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="G230" s="2"/>
       <c r="H230" s="1" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="I230" s="1" t="n">
         <v>28</v>
       </c>
       <c r="J230" s="0" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="2"/>
       <c r="B231" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>
       <c r="E231" s="2"/>
       <c r="F231" s="1" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="G231" s="1" t="n">
         <v>2110</v>
       </c>
       <c r="H231" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="I231" s="1" t="n">
         <v>29</v>
@@ -6054,19 +6066,19 @@
     <row r="232" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="2"/>
       <c r="B232" s="1" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
       <c r="E232" s="2"/>
       <c r="F232" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="G232" s="1" t="n">
         <v>2120</v>
       </c>
       <c r="H232" s="1" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="I232" s="1" t="n">
         <v>30</v>
@@ -6075,13 +6087,13 @@
     <row r="233" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="2"/>
       <c r="B233" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C233" s="2"/>
       <c r="D233" s="2"/>
       <c r="E233" s="2"/>
       <c r="F233" s="1" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="G233" s="1" t="n">
         <v>2130</v>
@@ -6094,13 +6106,13 @@
     <row r="234" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="2"/>
       <c r="B234" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C234" s="2"/>
       <c r="D234" s="2"/>
       <c r="E234" s="2"/>
       <c r="F234" s="1" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="G234" s="1" t="n">
         <v>2140</v>
@@ -6113,13 +6125,13 @@
     <row r="235" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="2"/>
       <c r="B235" s="1" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
       <c r="E235" s="2"/>
       <c r="F235" s="1" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="G235" s="1" t="n">
         <v>2150</v>
@@ -6132,13 +6144,13 @@
     <row r="236" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="2"/>
       <c r="B236" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
       <c r="E236" s="2"/>
       <c r="F236" s="1" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="G236" s="1" t="n">
         <v>2220</v>
@@ -6151,13 +6163,13 @@
     <row r="237" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="2"/>
       <c r="B237" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
       <c r="E237" s="2"/>
       <c r="F237" s="1" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="G237" s="1" t="n">
         <v>2300</v>
@@ -6170,13 +6182,13 @@
     <row r="238" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="2"/>
       <c r="B238" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
       <c r="F238" s="1" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="G238" s="1" t="n">
         <v>2400</v>
@@ -6210,40 +6222,40 @@
     </row>
     <row r="241" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
       <c r="D241" s="2"/>
       <c r="E241" s="2"/>
       <c r="F241" s="1" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="G241" s="2"/>
       <c r="H241" s="1" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="I241" s="1" t="n">
         <v>31</v>
       </c>
       <c r="J241" s="0" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="2"/>
       <c r="B242" s="1" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="C242" s="2"/>
       <c r="D242" s="2"/>
       <c r="E242" s="2"/>
       <c r="F242" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="G242" s="2"/>
       <c r="H242" s="1" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="I242" s="2"/>
     </row>
@@ -6251,12 +6263,12 @@
       <c r="A243" s="2"/>
       <c r="B243" s="2"/>
       <c r="C243" s="1" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="D243" s="2"/>
       <c r="E243" s="2"/>
       <c r="F243" s="1" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="G243" s="1" t="n">
         <v>3100</v>
@@ -6271,11 +6283,11 @@
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
       <c r="D244" s="1" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="E244" s="2"/>
       <c r="F244" s="1" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="G244" s="1" t="n">
         <v>3210</v>
@@ -6288,11 +6300,11 @@
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
       <c r="D245" s="1" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E245" s="2"/>
       <c r="F245" s="1" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="G245" s="1" t="n">
         <v>3221</v>
@@ -6305,11 +6317,11 @@
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
       <c r="D246" s="1" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="E246" s="2"/>
       <c r="F246" s="1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="G246" s="1" t="n">
         <v>3222</v>
@@ -6322,11 +6334,11 @@
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
       <c r="D247" s="1" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="E247" s="2"/>
       <c r="F247" s="1" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="G247" s="1" t="n">
         <v>3223</v>
@@ -6339,11 +6351,11 @@
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
       <c r="D248" s="1" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="E248" s="2"/>
       <c r="F248" s="1" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="G248" s="1" t="n">
         <v>3224</v>
@@ -6356,11 +6368,11 @@
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
       <c r="D249" s="1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="E249" s="2"/>
       <c r="F249" s="1" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="G249" s="1" t="n">
         <v>3231</v>
@@ -6373,11 +6385,11 @@
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
       <c r="D250" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="E250" s="2"/>
       <c r="F250" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="G250" s="1" t="n">
         <v>3232</v>
@@ -6390,11 +6402,11 @@
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
       <c r="D251" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E251" s="2"/>
       <c r="F251" s="1" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="G251" s="1" t="n">
         <v>3234</v>
@@ -6407,11 +6419,11 @@
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
       <c r="D252" s="1" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="E252" s="2"/>
       <c r="F252" s="1" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="G252" s="1" t="n">
         <v>3236</v>
@@ -6424,11 +6436,11 @@
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
       <c r="D253" s="1" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="E253" s="2"/>
       <c r="F253" s="1" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="G253" s="1" t="n">
         <v>3237</v>
@@ -6441,11 +6453,11 @@
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
       <c r="D254" s="1" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="E254" s="2"/>
       <c r="F254" s="1" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="G254" s="1" t="n">
         <v>3241</v>
@@ -6458,11 +6470,11 @@
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
       <c r="D255" s="1" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="E255" s="2"/>
       <c r="F255" s="1" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="G255" s="1" t="n">
         <v>3242</v>
@@ -6475,11 +6487,11 @@
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
       <c r="D256" s="1" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="E256" s="2"/>
       <c r="F256" s="1" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="G256" s="1" t="n">
         <v>3243</v>
@@ -6492,11 +6504,11 @@
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
       <c r="D257" s="1" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="E257" s="2"/>
       <c r="F257" s="1" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="G257" s="1" t="n">
         <v>3245</v>
@@ -6509,11 +6521,11 @@
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
       <c r="D258" s="1" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="E258" s="2"/>
       <c r="F258" s="1" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="G258" s="1" t="n">
         <v>3246</v>
@@ -6525,12 +6537,12 @@
       <c r="A259" s="2"/>
       <c r="B259" s="2"/>
       <c r="C259" s="1" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="D259" s="2"/>
       <c r="E259" s="2"/>
       <c r="F259" s="1" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="G259" s="2"/>
       <c r="H259" s="2"/>
@@ -6543,11 +6555,11 @@
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
       <c r="D260" s="1" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="E260" s="2"/>
       <c r="F260" s="1" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="G260" s="1" t="n">
         <v>5100</v>
@@ -6560,11 +6572,11 @@
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
       <c r="D261" s="1" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="E261" s="2"/>
       <c r="F261" s="1" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="G261" s="1" t="n">
         <v>5220</v>
@@ -6577,11 +6589,11 @@
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
       <c r="D262" s="1" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="E262" s="2"/>
       <c r="F262" s="1" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="G262" s="1" t="n">
         <v>5230</v>

</xml_diff>